<commit_message>
Data read from excel file using data providor
</commit_message>
<xml_diff>
--- a/resources/testdata/ExcelFiles/Reg_data.xlsx
+++ b/resources/testdata/ExcelFiles/Reg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#Projects\Nazn33n-magent-selenium-testng-datadriven\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411510C5-201A-48F4-AAD3-89A91C31BF11}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF28CC40-6C8C-45CF-A90D-2F64A3C0AD96}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12084" windowHeight="5640" xr2:uid="{8FC389E6-B423-468E-A42F-8836C69D5384}"/>
   </bookViews>
@@ -25,81 +25,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Naz@1235</t>
+  </si>
+  <si>
+    <t>Naz@1236</t>
+  </si>
+  <si>
+    <t>Naz@1237</t>
+  </si>
+  <si>
+    <t>Naz@1238</t>
+  </si>
+  <si>
+    <t>Fahima</t>
+  </si>
+  <si>
+    <t>Shidik</t>
+  </si>
+  <si>
+    <t>Sohela</t>
+  </si>
+  <si>
+    <t>Sami</t>
+  </si>
+  <si>
+    <t>Lopa</t>
+  </si>
+  <si>
+    <t>karim</t>
+  </si>
+  <si>
+    <t>Halima</t>
+  </si>
+  <si>
+    <t>kuddus</t>
+  </si>
+  <si>
+    <t>Fahima1@yopmail.com</t>
+  </si>
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Naz@1234</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Confirm Password</t>
-  </si>
-  <si>
-    <t>Rabeya</t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>ali@yopmail.com</t>
-  </si>
-  <si>
-    <t>ali1@yopmail.com</t>
-  </si>
-  <si>
-    <t>ali2@yopmail.com</t>
-  </si>
-  <si>
-    <t>ali3@yopmail.com</t>
-  </si>
-  <si>
-    <t>ali4@yopmail.com</t>
-  </si>
-  <si>
-    <t>Naz@1235</t>
-  </si>
-  <si>
-    <t>Naz@1236</t>
-  </si>
-  <si>
-    <t>Naz@1237</t>
-  </si>
-  <si>
-    <t>Naz@1238</t>
-  </si>
-  <si>
-    <t>Fahima</t>
-  </si>
-  <si>
-    <t>Shidik</t>
-  </si>
-  <si>
-    <t>Sohela</t>
-  </si>
-  <si>
-    <t>Sami</t>
-  </si>
-  <si>
-    <t>Lopa</t>
-  </si>
-  <si>
-    <t>karim</t>
-  </si>
-  <si>
-    <t>Halima</t>
-  </si>
-  <si>
-    <t>kuddus</t>
+    <t>Fahima2@yopmail.com</t>
+  </si>
+  <si>
+    <t>Fahima3@yopmail.com</t>
+  </si>
+  <si>
+    <t>Fahima4@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -144,9 +132,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,147 +452,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43131B9A-398D-4EED-9DEF-BB604774AC0C}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
-    <col min="12" max="12" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="psu@yopmail.com" xr:uid="{19C1D17C-F4CC-4016-B685-CF756A8E0787}"/>
-    <hyperlink ref="B2" r:id="rId2" display="Naz@1234" xr:uid="{48F0873D-5B1F-4687-9BBB-CFCE1466AEA2}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{54C291B1-0726-4EFC-A367-8FB1487F80FA}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{31FE46CE-B516-47D5-9D69-B8A6DC28C4DC}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{4CA665E0-6A57-495A-8977-D43F238E6235}"/>
-    <hyperlink ref="C3:C6" r:id="rId6" display="ali@yopmail.com" xr:uid="{E5B4189F-116D-4F07-8603-0A73C153CFA4}"/>
-    <hyperlink ref="C3" r:id="rId7" xr:uid="{12B986DF-0548-4460-BAD3-E274A420E639}"/>
-    <hyperlink ref="C4" r:id="rId8" xr:uid="{A2939819-9B12-48D4-B850-9BB29A8447EE}"/>
-    <hyperlink ref="C5" r:id="rId9" xr:uid="{34E337F3-7484-48E9-B05E-2E3038611862}"/>
-    <hyperlink ref="C6" r:id="rId10" xr:uid="{222475BA-8227-44E9-8A7F-42212944076F}"/>
-    <hyperlink ref="A3:A6" r:id="rId11" display="psu@yopmail.com" xr:uid="{6E7C142B-7975-497F-8727-B203BA812980}"/>
-    <hyperlink ref="B3:B6" r:id="rId12" display="Naz@1234" xr:uid="{A765CCFA-9A83-4E38-A375-CE2C23D910DF}"/>
-    <hyperlink ref="D3:D6" r:id="rId13" display="Naz@1234" xr:uid="{92C04062-FE0F-4941-80B3-3BC91F073D14}"/>
-    <hyperlink ref="E3:E6" r:id="rId14" display="Naz@1234" xr:uid="{11B567EF-857F-4E84-8A0F-1C0656B4A015}"/>
+    <hyperlink ref="A2:A5" r:id="rId1" display="psu@yopmail.com" xr:uid="{6E7C142B-7975-497F-8727-B203BA812980}"/>
+    <hyperlink ref="B2:B5" r:id="rId2" display="Naz@1234" xr:uid="{A765CCFA-9A83-4E38-A375-CE2C23D910DF}"/>
+    <hyperlink ref="D2:D5" r:id="rId3" display="Naz@1234" xr:uid="{11B567EF-857F-4E84-8A0F-1C0656B4A015}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{C6B421FC-DB9D-4DB9-91C3-2BBEA6B8848E}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{8A84A3E9-4E5D-4F8B-8643-33457D872D61}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{C9191931-EA1F-4CDD-A2FB-0338B28B6FEA}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{E9E863AE-DEBB-4674-9077-2089E0232CFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Read billing address data from excel
</commit_message>
<xml_diff>
--- a/resources/testdata/ExcelFiles/Reg_data.xlsx
+++ b/resources/testdata/ExcelFiles/Reg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#Projects\Nazn33n-magent-selenium-testng-datadriven\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF28CC40-6C8C-45CF-A90D-2F64A3C0AD96}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DED88F0-FDDB-47B6-B67F-7112A86FA3A6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12084" windowHeight="5640" xr2:uid="{8FC389E6-B423-468E-A42F-8836C69D5384}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Password</t>
   </si>
@@ -42,6 +42,33 @@
     <t>Naz@1235</t>
   </si>
   <si>
+    <t>Fahima</t>
+  </si>
+  <si>
+    <t>Shidik</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Fahima3@yopmail.com</t>
+  </si>
+  <si>
+    <t>Lima</t>
+  </si>
+  <si>
+    <t>Saraf</t>
+  </si>
+  <si>
+    <t>Kibra</t>
+  </si>
+  <si>
+    <t>Hakim</t>
+  </si>
+  <si>
+    <t>lima1@yopmail.com</t>
+  </si>
+  <si>
     <t>Naz@1236</t>
   </si>
   <si>
@@ -51,43 +78,64 @@
     <t>Naz@1238</t>
   </si>
   <si>
-    <t>Fahima</t>
-  </si>
-  <si>
-    <t>Shidik</t>
-  </si>
-  <si>
-    <t>Sohela</t>
-  </si>
-  <si>
-    <t>Sami</t>
-  </si>
-  <si>
-    <t>Lopa</t>
-  </si>
-  <si>
-    <t>karim</t>
-  </si>
-  <si>
-    <t>Halima</t>
-  </si>
-  <si>
-    <t>kuddus</t>
-  </si>
-  <si>
-    <t>Fahima1@yopmail.com</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Fahima2@yopmail.com</t>
-  </si>
-  <si>
-    <t>Fahima3@yopmail.com</t>
-  </si>
-  <si>
-    <t>Fahima4@yopmail.com</t>
+    <t>Naz@1239</t>
+  </si>
+  <si>
+    <t>Naz@1240</t>
+  </si>
+  <si>
+    <t>Naz@1241</t>
+  </si>
+  <si>
+    <t>Naz@1242</t>
+  </si>
+  <si>
+    <t>Naz@1243</t>
+  </si>
+  <si>
+    <t>Naz@1244</t>
+  </si>
+  <si>
+    <t>Fifa</t>
+  </si>
+  <si>
+    <t>kashem</t>
+  </si>
+  <si>
+    <t>Hero</t>
+  </si>
+  <si>
+    <t>Miro</t>
+  </si>
+  <si>
+    <t>Kilo</t>
+  </si>
+  <si>
+    <t>Chilo</t>
+  </si>
+  <si>
+    <t>Pilo</t>
+  </si>
+  <si>
+    <t>Kibra1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Fifa1@yopmail.com</t>
+  </si>
+  <si>
+    <t>kashem1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Hero1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Miro1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Kilo1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Pilo1@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -452,11 +500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43131B9A-398D-4EED-9DEF-BB604774AC0C}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +512,7 @@
     <col min="1" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="34.21875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" customWidth="1"/>
     <col min="10" max="10" width="13.44140625" customWidth="1"/>
     <col min="11" max="11" width="20.21875" customWidth="1"/>
@@ -478,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -489,71 +537,191 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2:A5" r:id="rId1" display="psu@yopmail.com" xr:uid="{6E7C142B-7975-497F-8727-B203BA812980}"/>
-    <hyperlink ref="B2:B5" r:id="rId2" display="Naz@1234" xr:uid="{A765CCFA-9A83-4E38-A375-CE2C23D910DF}"/>
-    <hyperlink ref="D2:D5" r:id="rId3" display="Naz@1234" xr:uid="{11B567EF-857F-4E84-8A0F-1C0656B4A015}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{C6B421FC-DB9D-4DB9-91C3-2BBEA6B8848E}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{8A84A3E9-4E5D-4F8B-8643-33457D872D61}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{C9191931-EA1F-4CDD-A2FB-0338B28B6FEA}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{E9E863AE-DEBB-4674-9077-2089E0232CFE}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{C6B421FC-DB9D-4DB9-91C3-2BBEA6B8848E}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{14E99ACC-413C-47D8-ACB2-3873C7E948BF}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{EF00CAE5-A0A6-4BEC-B788-29F792F24F76}"/>
+    <hyperlink ref="D3:D11" r:id="rId4" display="Naz@1235" xr:uid="{FEDADDF5-3928-4133-A2B2-E6C480F6C307}"/>
+    <hyperlink ref="C4:C11" r:id="rId5" display="lima1@yopmail.com" xr:uid="{1F76A04B-E110-47CD-936E-740BFFA57772}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{D239983B-196C-4A8E-A3E7-C104E782585B}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{1D7E3C3C-5EA1-4BEF-818D-11EE08DB841D}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{82777A0B-18DE-43CF-B060-AC35D8A2E708}"/>
+    <hyperlink ref="C7" r:id="rId9" xr:uid="{2433AB86-4C1A-48C8-A233-354FD670D2FC}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{CA5DDBBE-550E-4F94-BA67-5B0A28E38168}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{9D927913-0F68-4F12-94F0-C5AA8EEE641E}"/>
+    <hyperlink ref="C10" r:id="rId12" xr:uid="{699BFF3B-AD26-412F-BFE2-7A8A314D0B59}"/>
+    <hyperlink ref="C11" r:id="rId13" xr:uid="{B44CD1D8-2D0E-4B7E-A4FF-0DE67EE20E8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dynamic the menu, submenu and product
</commit_message>
<xml_diff>
--- a/resources/testdata/ExcelFiles/Reg_data.xlsx
+++ b/resources/testdata/ExcelFiles/Reg_data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#Projects\Nazn33n-magent-selenium-testng-datadriven\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAD07EA-50D1-4350-840D-14B4DFE49718}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FE316C-531D-42A6-AE0D-351F65092421}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12084" windowHeight="5640" xr2:uid="{8FC389E6-B423-468E-A42F-8836C69D5384}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>First Name</t>
   </si>
@@ -64,15 +64,46 @@
   </si>
   <si>
     <t>Nazz63@yopmail.com</t>
+  </si>
+  <si>
+    <t>Cloth Category</t>
+  </si>
+  <si>
+    <t>Men_Tops_Tees</t>
+  </si>
+  <si>
+    <t>Women_Bottoms_Pants</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -100,8 +131,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,66 +454,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96479B6-4D88-44F5-AD3A-C5DC70970BFC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3">
+        <v>28</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify excel and code
</commit_message>
<xml_diff>
--- a/resources/testdata/ExcelFiles/Reg_data.xlsx
+++ b/resources/testdata/ExcelFiles/Reg_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#Projects\Nazn33n-magent-selenium-testng-datadriven\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FE316C-531D-42A6-AE0D-351F65092421}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AC0CDF-92DB-428E-82C6-A88EAE701ABD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12084" windowHeight="5640" xr2:uid="{8FC389E6-B423-468E-A42F-8836C69D5384}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>First Name</t>
   </si>
@@ -42,36 +42,9 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Earl</t>
-  </si>
-  <si>
-    <t>Langosh</t>
-  </si>
-  <si>
-    <t>2TcX22zT@1</t>
-  </si>
-  <si>
-    <t>Nazz62@yopmail.com</t>
-  </si>
-  <si>
-    <t>Lyndon</t>
-  </si>
-  <si>
-    <t>O'Hara</t>
-  </si>
-  <si>
-    <t>K53Thskv@1</t>
-  </si>
-  <si>
-    <t>Nazz63@yopmail.com</t>
-  </si>
-  <si>
     <t>Cloth Category</t>
   </si>
   <si>
-    <t>Men_Tops_Tees</t>
-  </si>
-  <si>
     <t>Women_Bottoms_Pants</t>
   </si>
   <si>
@@ -81,13 +54,49 @@
     <t>Color</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
     <t>Blue</t>
   </si>
   <si>
-    <t>M</t>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>Gulshan, Police Plaza</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Nazneen's Software Company</t>
+  </si>
+  <si>
+    <t>Buckridge</t>
+  </si>
+  <si>
+    <t>Rafael</t>
+  </si>
+  <si>
+    <t>Nazz72@yopmail.com</t>
+  </si>
+  <si>
+    <t>szMYqE9k@1</t>
   </si>
 </sst>
 </file>
@@ -131,15 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,20 +457,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96479B6-4D88-44F5-AD3A-C5DC70970BFC}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
+    <col min="11" max="11" width="15.21875" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,78 +486,91 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>1546745564</v>
+      </c>
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2">
+        <v>1215</v>
+      </c>
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="M2">
         <v>28</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="N2" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="ahsGmLIT@1" xr:uid="{68B0B562-5CEE-4007-B98B-607BFD7214A9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dynamic the product, size and color. Also placed the order
</commit_message>
<xml_diff>
--- a/resources/testdata/ExcelFiles/Reg_data.xlsx
+++ b/resources/testdata/ExcelFiles/Reg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#Projects\Nazn33n-magent-selenium-testng-datadriven\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AC0CDF-92DB-428E-82C6-A88EAE701ABD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A192B76A-2918-45AB-82E8-A49AE80E51AE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12084" windowHeight="5640" xr2:uid="{8FC389E6-B423-468E-A42F-8836C69D5384}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
     <t>Street Address</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>szMYqE9k@1</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
@@ -460,22 +460,25 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" customWidth="1"/>
-    <col min="11" max="11" width="15.21875" customWidth="1"/>
-    <col min="12" max="12" width="22" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -495,22 +498,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -524,34 +527,34 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>1546745564</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2">
         <v>1215</v>
@@ -560,10 +563,10 @@
         <v>6</v>
       </c>
       <c r="M2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>